<commit_message>
adding in tests for default padding (and a test to make sure padding works). rspec breaks on tyhpheous gem -- comment out in spec_helper to get excelx spec to run
</commit_message>
<xml_diff>
--- a/test/files/numbers1.xlsx
+++ b/test/files/numbers1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="2400" windowWidth="16380" windowHeight="8200" tabRatio="344" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="2740" yWindow="2400" windowWidth="22660" windowHeight="14480" tabRatio="471" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="130000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -79,16 +79,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -117,20 +112,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -477,15 +472,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1">
@@ -636,7 +630,7 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -644,15 +638,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="5" spans="2:5">
       <c r="C5" t="s">
@@ -681,7 +674,7 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -689,15 +682,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA1"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:53">
       <c r="A1" t="s">
@@ -720,7 +712,7 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -728,15 +720,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2">
@@ -762,7 +753,7 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -770,15 +761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
@@ -867,7 +857,7 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Added support to return integer value.
</commit_message>
<xml_diff>
--- a/test/files/numbers1.xlsx
+++ b/test/files/numbers1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="2400" windowWidth="22660" windowHeight="14480" tabRatio="471" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="471" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -114,12 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,10 +719,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -744,6 +742,17 @@
       </c>
       <c r="E1">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1234</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1234</v>
+      </c>
+      <c r="C3">
+        <v>1234.1199999999999</v>
       </c>
     </row>
   </sheetData>
@@ -764,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>